<commit_message>
Se agrego el enlace al MIRO y se modifico el artículo personal al igual que el excel de categorizacion de revistas
</commit_message>
<xml_diff>
--- a/Entrega/EV9/Categorización Revistas.xlsx
+++ b/Entrega/EV9/Categorización Revistas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\complementario-3125033\04-Sesión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\complementario-3125033\Entrega\EV9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B84CBD2-1DD3-4E9B-8EDF-853191A522C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA597352-BAFB-4C8D-B206-8D571E23ACAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D569174F-4A60-4622-86E0-BC10BDE4ABDE}"/>
   </bookViews>
@@ -211,7 +211,7 @@
   </si>
   <si>
     <t>A traves de la busqueda de revistas en las cuales podria publicar mi artículo, he optado por publicarlo en la revista del SENA, 
-puesto que es mejor y mas facil, ya que al ser parte del SENA tendría acceso directo a recursos y soporte que facilitarían la publicación de mi trabajo, a parte de ser gratis no tendría costos adicionales.</t>
+puesto que es mejor y mas facil, ya que al ser parte del SENA tendría acceso directo a recursos y soporte que facilitarían la publicación de mi trabajo, a parte de ser gratis no tendría costos adicionales, igualmente a ser una revista no categorizada, no se requiere mucho para subir mi artículo</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,7 +926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>

</xml_diff>